<commit_message>
Reduced number of variable cards and increased the number of repetition cards.
</commit_message>
<xml_diff>
--- a/development/Card Frequncies.xlsx
+++ b/development/Card Frequncies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Instruction</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Number of Cards / Player</t>
+  </si>
+  <si>
+    <t>Total Cards</t>
   </si>
 </sst>
 </file>
@@ -149,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -403,6 +406,15 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -414,7 +426,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -453,12 +465,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,12 +487,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -602,6 +602,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -889,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,11 +930,11 @@
       <c r="B1" s="2">
         <v>5</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="53" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="49" t="s">
         <v>13</v>
       </c>
     </row>
@@ -926,15 +945,15 @@
       <c r="B2" s="2">
         <v>10</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="9">
         <v>1</v>
       </c>
-      <c r="F2" s="54">
+      <c r="F2" s="50">
         <f>$B$3*'Card Frequencies'!C3</f>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -945,202 +964,216 @@
         <f>B1*B2</f>
         <v>50</v>
       </c>
-      <c r="D3" s="30"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="9">
         <v>2</v>
       </c>
-      <c r="F3" s="54">
+      <c r="F3" s="50">
         <f>$B$3*'Card Frequencies'!C4</f>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="30"/>
+      <c r="D4" s="26"/>
       <c r="E4" s="9">
         <v>3</v>
       </c>
-      <c r="F4" s="54">
+      <c r="F4" s="50">
         <f>$B$3*'Card Frequencies'!C5</f>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="30"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="9">
         <v>4</v>
       </c>
-      <c r="F5" s="54">
+      <c r="F5" s="50">
         <f>$B$3*'Card Frequencies'!C6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="36">
+        <v>2</v>
+      </c>
+      <c r="F6" s="51">
+        <f>$B$3*'Card Frequencies'!E4</f>
+        <v>1.1111111111111112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="27"/>
+      <c r="E7" s="28">
+        <v>3</v>
+      </c>
+      <c r="F7" s="52">
+        <f>$B$3*'Card Frequencies'!E5</f>
+        <v>2.2222222222222223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="27"/>
+      <c r="E8" s="28">
+        <v>4</v>
+      </c>
+      <c r="F8" s="52">
+        <f>$B$3*'Card Frequencies'!E6</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="27"/>
+      <c r="E9" s="28">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="40">
+      <c r="F9" s="52">
+        <f>$B$3*'Card Frequencies'!E7</f>
+        <v>2.2222222222222223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="27"/>
+      <c r="E10" s="28">
+        <v>6</v>
+      </c>
+      <c r="F10" s="52">
+        <f>$B$3*'Card Frequencies'!E8</f>
+        <v>1.1111111111111112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="27"/>
+      <c r="E11" s="28">
+        <v>7</v>
+      </c>
+      <c r="F11" s="52">
+        <f>$B$3*'Card Frequencies'!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="37"/>
+      <c r="E12" s="38">
+        <v>8</v>
+      </c>
+      <c r="F12" s="53">
+        <f>$B$3*'Card Frequencies'!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="55">
-        <f>$B$3*'Card Frequencies'!E4</f>
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="31"/>
-      <c r="E7" s="32">
+      <c r="E13" s="40">
+        <v>2</v>
+      </c>
+      <c r="F13" s="54">
+        <f>$B$3*'Card Frequencies'!G4</f>
+        <v>4.1666666666666661</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="29"/>
+      <c r="E14" s="30">
         <v>3</v>
       </c>
-      <c r="F7" s="56">
-        <f>$B$3*'Card Frequencies'!E5</f>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="31"/>
-      <c r="E8" s="32">
+      <c r="F14" s="55">
+        <f>$B$3*'Card Frequencies'!G5</f>
+        <v>4.1666666666666661</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="29"/>
+      <c r="E15" s="30">
         <v>4</v>
       </c>
-      <c r="F8" s="56">
-        <f>$B$3*'Card Frequencies'!E6</f>
-        <v>1.8750000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="31"/>
-      <c r="E9" s="32">
-        <v>5</v>
-      </c>
-      <c r="F9" s="56">
-        <f>$B$3*'Card Frequencies'!E7</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="31"/>
-      <c r="E10" s="32">
-        <v>6</v>
-      </c>
-      <c r="F10" s="56">
-        <f>$B$3*'Card Frequencies'!E8</f>
-        <v>1.8750000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="31"/>
-      <c r="E11" s="32">
-        <v>7</v>
-      </c>
-      <c r="F11" s="56">
-        <f>$B$3*'Card Frequencies'!E9</f>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="41"/>
-      <c r="E12" s="42">
+      <c r="F15" s="55">
+        <f>$B$3*'Card Frequencies'!G6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="41"/>
+      <c r="E16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="57">
-        <f>$B$3*'Card Frequencies'!E10</f>
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="43" t="s">
+      <c r="F16" s="56">
+        <f>$B$3*'Card Frequencies'!G7</f>
+        <v>4.1666666666666661</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="44">
         <v>2</v>
       </c>
-      <c r="E13" s="44">
-        <v>2</v>
-      </c>
-      <c r="F13" s="58">
-        <f>$B$3*'Card Frequencies'!G4</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="33"/>
-      <c r="E14" s="34">
+      <c r="F17" s="57">
+        <f>$B$3*'Card Frequencies'!I4</f>
+        <v>2.0000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="31"/>
+      <c r="E18" s="32">
         <v>3</v>
       </c>
-      <c r="F14" s="59">
-        <f>$B$3*'Card Frequencies'!G5</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="33"/>
-      <c r="E15" s="34">
+      <c r="F18" s="58">
+        <f>$B$3*'Card Frequencies'!I5</f>
+        <v>2.0000000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="45"/>
+      <c r="E19" s="46">
         <v>4</v>
       </c>
-      <c r="F15" s="59">
-        <f>$B$3*'Card Frequencies'!G6</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="45"/>
-      <c r="E16" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="60">
-        <f>$B$3*'Card Frequencies'!G7</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="48">
-        <v>2</v>
-      </c>
-      <c r="F17" s="61">
-        <f>$B$3*'Card Frequencies'!I4</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="35"/>
-      <c r="E18" s="36">
-        <v>3</v>
-      </c>
-      <c r="F18" s="62">
-        <f>$B$3*'Card Frequencies'!I5</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="49"/>
-      <c r="E19" s="50">
+      <c r="F19" s="59">
+        <f>$B$3*'Card Frequencies'!I6</f>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="63">
-        <f>$B$3*'Card Frequencies'!I6</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="64">
+      <c r="E20" s="34"/>
+      <c r="F20" s="60">
         <f>B3*'Card Frequencies'!J11</f>
         <v>2.5</v>
       </c>
     </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="63"/>
+      <c r="F21" s="61">
+        <f>SUM(F2:F20)</f>
+        <v>49.999999999999993</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D21:E21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,23 +1190,23 @@
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="65"/>
+      <c r="D1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="65"/>
+      <c r="F1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="65"/>
+      <c r="H1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="20" t="s">
+      <c r="I1" s="65"/>
+      <c r="J1" s="18" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="7" t="s">
@@ -1184,230 +1217,210 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24">
+      <c r="B2" s="66">
         <v>0.4</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="24">
+      <c r="C2" s="67"/>
+      <c r="D2" s="66">
         <v>0.2</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="24">
-        <v>0.2</v>
-      </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="24">
-        <v>0.15</v>
-      </c>
-      <c r="J2" s="26">
+      <c r="E2" s="67"/>
+      <c r="F2" s="66">
+        <v>0.25</v>
+      </c>
+      <c r="G2" s="67"/>
+      <c r="H2" s="66">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="67"/>
+      <c r="J2" s="22">
         <v>0.05</v>
       </c>
       <c r="K2" s="6">
-        <f>SUM(C2:J2)</f>
+        <f>SUM(B2:J2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
       <c r="C3" s="11">
-        <f>$C$2/COUNT($B$3:$B6)</f>
-        <v>0.1</v>
-      </c>
-      <c r="D3" s="16"/>
+        <f>$B$2/COUNT($B$3:$B6)</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="D3" s="14"/>
       <c r="E3" s="12"/>
-      <c r="F3" s="16"/>
+      <c r="F3" s="14"/>
       <c r="G3" s="12"/>
-      <c r="H3" s="16"/>
+      <c r="H3" s="14"/>
       <c r="I3" s="12"/>
-      <c r="J3" s="21"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="16">
+      <c r="B4" s="14">
         <v>2</v>
       </c>
       <c r="C4" s="11">
-        <f>$C$2/COUNT($B$3:$B7)</f>
-        <v>0.1</v>
-      </c>
-      <c r="D4" s="16">
+        <f>$B$2/COUNT($B$3:$B7)</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="D4" s="14">
         <v>2</v>
       </c>
       <c r="E4" s="13">
-        <f>$E$2/16</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="F4" s="16">
+        <f>$D$2/9</f>
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="F4" s="14">
         <v>2</v>
       </c>
       <c r="G4" s="13">
-        <f>$G$2/(COUNT(F:F)+1)</f>
-        <v>0.05</v>
-      </c>
-      <c r="H4" s="16">
+        <f>$F$2/(COUNT(F:F))</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H4" s="14">
         <v>2</v>
       </c>
       <c r="I4" s="13">
-        <f>$I$2*0.4</f>
-        <v>0.06</v>
-      </c>
-      <c r="J4" s="21"/>
+        <f>$H$2*0.4</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="16">
+      <c r="B5" s="14">
         <v>3</v>
       </c>
       <c r="C5" s="11">
-        <f>$C$2/COUNT($B$3:$B8)</f>
-        <v>0.1</v>
-      </c>
-      <c r="D5" s="16">
+        <f>$B$2/COUNT($B$3:$B8)</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="D5" s="14">
         <v>3</v>
       </c>
       <c r="E5" s="13">
-        <f>$E$2/16*2</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F5" s="16">
+        <f>$D$2/9*2</f>
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="F5" s="14">
         <v>3</v>
       </c>
       <c r="G5" s="13">
-        <f>$G$2/(COUNT(F:F)+1)</f>
-        <v>0.05</v>
-      </c>
-      <c r="H5" s="16">
+        <f t="shared" ref="G5:G7" si="0">$F$2/(COUNT(F:F))</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H5" s="14">
         <v>3</v>
       </c>
       <c r="I5" s="13">
-        <f>$I$2*0.4</f>
-        <v>0.06</v>
-      </c>
-      <c r="J5" s="21"/>
+        <f>$H$2*0.4</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="16">
+      <c r="B6" s="14"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="14">
         <v>4</v>
       </c>
-      <c r="C6" s="11">
-        <f>$C$2/COUNT(B:B)</f>
-        <v>0.1</v>
-      </c>
-      <c r="D6" s="16">
+      <c r="E6" s="13">
+        <f>$D$2/9*3</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14">
         <v>4</v>
       </c>
-      <c r="E6" s="13">
-        <f>$E$2/16*3</f>
-        <v>3.7500000000000006E-2</v>
-      </c>
-      <c r="F6" s="16">
-        <v>4</v>
-      </c>
-      <c r="G6" s="13">
-        <f>$G$2/(COUNT(F:F)+1)</f>
-        <v>0.05</v>
-      </c>
-      <c r="H6" s="16">
-        <v>4</v>
-      </c>
       <c r="I6" s="13">
-        <f>$I$2*0.2</f>
-        <v>0.03</v>
-      </c>
-      <c r="J6" s="21"/>
+        <f>$H$2*0.2</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="16"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="12"/>
-      <c r="D7" s="16">
+      <c r="D7" s="14">
         <v>5</v>
       </c>
       <c r="E7" s="13">
-        <f>$E$2/16*4</f>
-        <v>0.05</v>
-      </c>
-      <c r="F7" s="16" t="s">
+        <f>$D$2/9*2</f>
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="13">
-        <f>$G$2/(COUNT(F:F)+1)</f>
-        <v>0.05</v>
-      </c>
-      <c r="H7" s="16"/>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H7" s="14"/>
       <c r="I7" s="12"/>
-      <c r="J7" s="21"/>
+      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="12"/>
-      <c r="D8" s="16">
+      <c r="D8" s="14">
         <v>6</v>
       </c>
       <c r="E8" s="13">
-        <f>$E$2/16*3</f>
-        <v>3.7500000000000006E-2</v>
-      </c>
-      <c r="F8" s="16"/>
+        <f>$D$2/9*1</f>
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="F8" s="14"/>
       <c r="G8" s="12"/>
-      <c r="H8" s="16"/>
+      <c r="H8" s="14"/>
       <c r="I8" s="12"/>
-      <c r="J8" s="21"/>
+      <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="16"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="12"/>
-      <c r="D9" s="16">
-        <v>7</v>
-      </c>
-      <c r="E9" s="13">
-        <f>$E$2/16*2</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F9" s="16"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="16"/>
+      <c r="H9" s="14"/>
       <c r="I9" s="12"/>
-      <c r="J9" s="21"/>
+      <c r="J9" s="19"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="23">
-        <v>8</v>
-      </c>
-      <c r="E10" s="28">
-        <f>$E$2/16</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="29"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="25"/>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="17"/>
-      <c r="C11" s="18">
+      <c r="B11" s="15"/>
+      <c r="C11" s="16">
         <f>SUM(C3:C10)</f>
         <v>0.4</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="18">
+      <c r="D11" s="17"/>
+      <c r="E11" s="16">
         <f>SUM(E3:E10)</f>
         <v>0.2</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="18">
+      <c r="F11" s="17"/>
+      <c r="G11" s="16">
         <f>SUM(G3:G10)</f>
-        <v>0.2</v>
-      </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="16">
         <f>SUM(I3:I10)</f>
-        <v>0.15</v>
-      </c>
-      <c r="J11" s="22">
+        <v>0.10000000000000002</v>
+      </c>
+      <c r="J11" s="20">
         <v>0.05</v>
       </c>
       <c r="K11" s="8">
@@ -1415,12 +1428,19 @@
         <v>1</v>
       </c>
     </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="62"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>